<commit_message>
[TASK] Does more testing
</commit_message>
<xml_diff>
--- a/Experiments/TicTacToe/log.xlsx
+++ b/Experiments/TicTacToe/log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Mut</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>stagniert bei 0.3 rating ab 45 M Comp.</t>
+  </si>
+  <si>
+    <t>nach ca 40 M Comp. =&gt; 1.0 rating</t>
+  </si>
+  <si>
+    <t>nach ca 80 M Comp. =&gt; 0.99 rating</t>
+  </si>
+  <si>
+    <t>nach ca 10 M Comp. =&gt; stagnation 0.5 rating</t>
+  </si>
+  <si>
+    <t>nach ca 38 M Comp. =&gt; 1.0 rating</t>
+  </si>
+  <si>
+    <t>nach ca 60 M Comp. =&gt; 1.0 rating</t>
   </si>
 </sst>
 </file>
@@ -396,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -646,6 +661,118 @@
       </c>
       <c r="G11" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B12">
+        <v>0.3</v>
+      </c>
+      <c r="C12">
+        <v>200</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B13">
+        <v>0.3</v>
+      </c>
+      <c r="C13">
+        <v>150</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B14">
+        <v>0.3</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B15">
+        <v>0.3</v>
+      </c>
+      <c r="C15">
+        <v>300</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B16">
+        <v>0.3</v>
+      </c>
+      <c r="C16">
+        <v>350</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Adds more preferences to the tictactoe example
</commit_message>
<xml_diff>
--- a/Experiments/TicTacToe/log.xlsx
+++ b/Experiments/TicTacToe/log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Mut</t>
   </si>
@@ -79,6 +79,27 @@
   </si>
   <si>
     <t>nach ca 60 M Comp. =&gt; 1.0 rating</t>
+  </si>
+  <si>
+    <t>nach ca 50 M Comp. =&gt; 1.0 rating</t>
+  </si>
+  <si>
+    <t>nach ca 30 M Comp. =&gt; 1.0 rating</t>
+  </si>
+  <si>
+    <t>N in 1. L</t>
+  </si>
+  <si>
+    <t>N in 2. L</t>
+  </si>
+  <si>
+    <t>nach ca 25 M Comp. =&gt; 1.0 rating (8 min)</t>
+  </si>
+  <si>
+    <t>nach ca 75 M Comp. =&gt; 1.0 rating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nach ca 63 M Comp. =&gt; 1.0 rating </t>
   </si>
 </sst>
 </file>
@@ -411,18 +432,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="7" max="7" width="71.77734375" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="59.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,8 +463,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>1.8</v>
       </c>
@@ -461,11 +489,17 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1.8</v>
       </c>
@@ -481,11 +515,17 @@
       <c r="E3">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>1.8</v>
       </c>
@@ -501,11 +541,17 @@
       <c r="E4">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>1.8</v>
       </c>
@@ -524,11 +570,17 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>1.8</v>
       </c>
@@ -547,11 +599,17 @@
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>1.8</v>
       </c>
@@ -567,11 +625,17 @@
       <c r="E7">
         <v>10</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -590,11 +654,17 @@
       <c r="F8">
         <v>4</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -613,11 +683,17 @@
       <c r="F9">
         <v>5</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>0.3</v>
       </c>
@@ -636,11 +712,17 @@
       <c r="F10">
         <v>6</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>0.01</v>
       </c>
@@ -659,11 +741,17 @@
       <c r="F11">
         <v>7</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>1.8</v>
       </c>
@@ -682,11 +770,17 @@
       <c r="F12">
         <v>8</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>1.8</v>
       </c>
@@ -705,11 +799,17 @@
       <c r="F13">
         <v>9</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>1.8</v>
       </c>
@@ -725,11 +825,17 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>1.8</v>
       </c>
@@ -748,11 +854,17 @@
       <c r="F15">
         <v>10</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>1.8</v>
       </c>
@@ -771,8 +883,280 @@
       <c r="F16">
         <v>11</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B17">
+        <v>0.3</v>
+      </c>
+      <c r="C17">
+        <v>250</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B18">
+        <v>0.3</v>
+      </c>
+      <c r="C18">
+        <v>250</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B19">
+        <v>0.3</v>
+      </c>
+      <c r="C19">
+        <v>250</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>12</v>
+      </c>
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B20">
+        <v>0.3</v>
+      </c>
+      <c r="C20">
+        <v>250</v>
+      </c>
+      <c r="D20">
+        <v>25</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B21">
+        <v>0.3</v>
+      </c>
+      <c r="C21">
+        <v>250</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B22">
+        <v>0.3</v>
+      </c>
+      <c r="C22">
+        <v>250</v>
+      </c>
+      <c r="D22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>9</v>
+      </c>
+      <c r="H22">
+        <v>9</v>
+      </c>
+      <c r="I22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B23">
+        <v>0.3</v>
+      </c>
+      <c r="C23">
+        <v>250</v>
+      </c>
+      <c r="D23">
+        <v>25</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>13</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+      <c r="I23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B24">
+        <v>0.3</v>
+      </c>
+      <c r="C24">
+        <v>250</v>
+      </c>
+      <c r="D24">
+        <v>25</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B25">
+        <v>0.3</v>
+      </c>
+      <c r="C25">
+        <v>250</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B26">
+        <v>0.3</v>
+      </c>
+      <c r="C26">
+        <v>250</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Adds boolean preferences
</commit_message>
<xml_diff>
--- a/Experiments/TicTacToe/log.xlsx
+++ b/Experiments/TicTacToe/log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Mut</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t xml:space="preserve">nach ca 63 M Comp. =&gt; 1.0 rating </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nach ca 64 M Comp. =&gt; 1.0 rating </t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1157,6 +1160,32 @@
       </c>
       <c r="I26" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B27">
+        <v>0.3</v>
+      </c>
+      <c r="C27">
+        <v>250</v>
+      </c>
+      <c r="D27">
+        <v>25</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Makes sure all observers are removed when closing a sub app window
</commit_message>
<xml_diff>
--- a/Experiments/TicTacToe/log.xlsx
+++ b/Experiments/TicTacToe/log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
   <si>
     <t>Mut</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t xml:space="preserve">nach ca 64 M Comp. =&gt; 1.0 rating </t>
+  </si>
+  <si>
+    <t>Shortcuts</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nach ca 58 M Comp. =&gt; 1.0 rating </t>
   </si>
 </sst>
 </file>
@@ -435,19 +447,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="59.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="10" max="10" width="69.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,8 +485,11 @@
       <c r="H1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>1.8</v>
       </c>
@@ -499,10 +515,13 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1.8</v>
       </c>
@@ -525,10 +544,13 @@
         <v>10</v>
       </c>
       <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>1.8</v>
       </c>
@@ -551,10 +573,13 @@
         <v>10</v>
       </c>
       <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>1.8</v>
       </c>
@@ -580,10 +605,13 @@
         <v>10</v>
       </c>
       <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>1.8</v>
       </c>
@@ -609,10 +637,13 @@
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>1.8</v>
       </c>
@@ -635,10 +666,13 @@
         <v>10</v>
       </c>
       <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -664,10 +698,13 @@
         <v>10</v>
       </c>
       <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -693,10 +730,13 @@
         <v>10</v>
       </c>
       <c r="I9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>0.3</v>
       </c>
@@ -722,10 +762,13 @@
         <v>10</v>
       </c>
       <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>0.01</v>
       </c>
@@ -751,10 +794,13 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>1.8</v>
       </c>
@@ -780,10 +826,13 @@
         <v>10</v>
       </c>
       <c r="I12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>1.8</v>
       </c>
@@ -809,10 +858,13 @@
         <v>10</v>
       </c>
       <c r="I13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>1.8</v>
       </c>
@@ -835,10 +887,13 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>1.8</v>
       </c>
@@ -864,10 +919,13 @@
         <v>10</v>
       </c>
       <c r="I15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>1.8</v>
       </c>
@@ -893,10 +951,13 @@
         <v>10</v>
       </c>
       <c r="I16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>1.8</v>
       </c>
@@ -919,10 +980,13 @@
         <v>10</v>
       </c>
       <c r="I17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>1.8</v>
       </c>
@@ -945,10 +1009,13 @@
         <v>10</v>
       </c>
       <c r="I18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>1.8</v>
       </c>
@@ -974,10 +1041,13 @@
         <v>10</v>
       </c>
       <c r="I19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>1.8</v>
       </c>
@@ -1000,10 +1070,13 @@
         <v>10</v>
       </c>
       <c r="I20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>1.8</v>
       </c>
@@ -1026,10 +1099,13 @@
         <v>10</v>
       </c>
       <c r="I21" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>1.8</v>
       </c>
@@ -1052,10 +1128,13 @@
         <v>9</v>
       </c>
       <c r="I22" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>1.8</v>
       </c>
@@ -1081,10 +1160,13 @@
         <v>5</v>
       </c>
       <c r="I23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>30</v>
+      </c>
+      <c r="J23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>1.8</v>
       </c>
@@ -1107,10 +1189,13 @@
         <v>3</v>
       </c>
       <c r="I24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>1.8</v>
       </c>
@@ -1133,10 +1218,13 @@
         <v>3</v>
       </c>
       <c r="I25" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>1.8</v>
       </c>
@@ -1159,10 +1247,13 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>1.8</v>
       </c>
@@ -1185,7 +1276,39 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B28">
+        <v>0.3</v>
+      </c>
+      <c r="C28">
+        <v>250</v>
+      </c>
+      <c r="D28">
+        <v>25</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>20</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[TASK] Makes the tc problem working
</commit_message>
<xml_diff>
--- a/Experiments/TicTacToe/log.xlsx
+++ b/Experiments/TicTacToe/log.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Documents\Visual Studio 2015\Projects\LightBulb\Experiments\TicTacToe\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="22116" windowHeight="9528"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Mut</t>
   </si>
@@ -115,13 +120,31 @@
   </si>
   <si>
     <t xml:space="preserve">nach ca 58 M Comp. =&gt; 1.0 rating </t>
+  </si>
+  <si>
+    <t>Mutationstrength</t>
+  </si>
+  <si>
+    <t>Weight decay fac</t>
+  </si>
+  <si>
+    <t>Create up to</t>
+  </si>
+  <si>
+    <t>nach ca 52 M Comp. Mit minimaler neuron count =&gt; 1.0 rating</t>
+  </si>
+  <si>
+    <t>nach ca 70 M Comp. Mit minimaler neuron count =&gt; 1.0 rating</t>
+  </si>
+  <si>
+    <t>nach ca 47 M Comp. Mit minimaler neuron count =&gt; 1.0 rating</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,13 +182,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -203,9 +234,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,9 +268,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,9 +303,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,21 +479,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
     <col min="9" max="9" width="9.33203125" customWidth="1"/>
-    <col min="10" max="10" width="69.88671875" customWidth="1"/>
+    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,8 +523,17 @@
       <c r="I1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1.8</v>
       </c>
@@ -517,11 +561,20 @@
       <c r="I2" t="s">
         <v>30</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2">
+        <v>1.6</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>250</v>
+      </c>
+      <c r="M2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1.8</v>
       </c>
@@ -546,11 +599,20 @@
       <c r="I3" t="s">
         <v>30</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3">
+        <v>1.6</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>250</v>
+      </c>
+      <c r="M3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1.8</v>
       </c>
@@ -575,11 +637,20 @@
       <c r="I4" t="s">
         <v>30</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4">
+        <v>1.6</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>250</v>
+      </c>
+      <c r="M4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1.8</v>
       </c>
@@ -607,11 +678,20 @@
       <c r="I5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5">
+        <v>1.6</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>250</v>
+      </c>
+      <c r="M5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1.8</v>
       </c>
@@ -639,11 +719,20 @@
       <c r="I6" t="s">
         <v>30</v>
       </c>
-      <c r="J6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6">
+        <v>1.6</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>250</v>
+      </c>
+      <c r="M6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1.8</v>
       </c>
@@ -668,11 +757,20 @@
       <c r="I7" t="s">
         <v>30</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7">
+        <v>1.6</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>250</v>
+      </c>
+      <c r="M7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -700,11 +798,20 @@
       <c r="I8" t="s">
         <v>30</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8">
+        <v>1.6</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>250</v>
+      </c>
+      <c r="M8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -732,11 +839,20 @@
       <c r="I9" t="s">
         <v>30</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9">
+        <v>1.6</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>250</v>
+      </c>
+      <c r="M9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.3</v>
       </c>
@@ -764,11 +880,20 @@
       <c r="I10" t="s">
         <v>30</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10">
+        <v>1.6</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>250</v>
+      </c>
+      <c r="M10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>0.01</v>
       </c>
@@ -796,11 +921,20 @@
       <c r="I11" t="s">
         <v>30</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11">
+        <v>1.6</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>250</v>
+      </c>
+      <c r="M11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1.8</v>
       </c>
@@ -828,11 +962,20 @@
       <c r="I12" t="s">
         <v>30</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12">
+        <v>1.6</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>250</v>
+      </c>
+      <c r="M12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1.8</v>
       </c>
@@ -860,11 +1003,20 @@
       <c r="I13" t="s">
         <v>30</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13">
+        <v>1.6</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>250</v>
+      </c>
+      <c r="M13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1.8</v>
       </c>
@@ -889,11 +1041,20 @@
       <c r="I14" t="s">
         <v>30</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14">
+        <v>1.6</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>250</v>
+      </c>
+      <c r="M14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1.8</v>
       </c>
@@ -921,11 +1082,20 @@
       <c r="I15" t="s">
         <v>30</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15">
+        <v>1.6</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>250</v>
+      </c>
+      <c r="M15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1.8</v>
       </c>
@@ -953,11 +1123,20 @@
       <c r="I16" t="s">
         <v>30</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16">
+        <v>1.6</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>250</v>
+      </c>
+      <c r="M16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1.8</v>
       </c>
@@ -982,11 +1161,20 @@
       <c r="I17" t="s">
         <v>30</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17">
+        <v>1.6</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>250</v>
+      </c>
+      <c r="M17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1.8</v>
       </c>
@@ -1011,11 +1199,20 @@
       <c r="I18" t="s">
         <v>30</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18">
+        <v>1.6</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>250</v>
+      </c>
+      <c r="M18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1.8</v>
       </c>
@@ -1043,11 +1240,20 @@
       <c r="I19" t="s">
         <v>30</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19">
+        <v>1.6</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>250</v>
+      </c>
+      <c r="M19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1.8</v>
       </c>
@@ -1072,11 +1278,20 @@
       <c r="I20" t="s">
         <v>30</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20">
+        <v>1.6</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>250</v>
+      </c>
+      <c r="M20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1.8</v>
       </c>
@@ -1101,11 +1316,20 @@
       <c r="I21" t="s">
         <v>30</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21">
+        <v>1.6</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>250</v>
+      </c>
+      <c r="M21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1.8</v>
       </c>
@@ -1130,11 +1354,20 @@
       <c r="I22" t="s">
         <v>30</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22">
+        <v>1.6</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>250</v>
+      </c>
+      <c r="M22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1.8</v>
       </c>
@@ -1162,11 +1395,20 @@
       <c r="I23" t="s">
         <v>30</v>
       </c>
-      <c r="J23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="J23">
+        <v>1.6</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>250</v>
+      </c>
+      <c r="M23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1.8</v>
       </c>
@@ -1191,11 +1433,20 @@
       <c r="I24" t="s">
         <v>30</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24">
+        <v>1.6</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>250</v>
+      </c>
+      <c r="M24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1.8</v>
       </c>
@@ -1220,11 +1471,20 @@
       <c r="I25" t="s">
         <v>30</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25">
+        <v>1.6</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>250</v>
+      </c>
+      <c r="M25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1.8</v>
       </c>
@@ -1249,11 +1509,20 @@
       <c r="I26" t="s">
         <v>30</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26">
+        <v>1.6</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>250</v>
+      </c>
+      <c r="M26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1.8</v>
       </c>
@@ -1278,11 +1547,20 @@
       <c r="I27" t="s">
         <v>30</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27">
+        <v>1.6</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>250</v>
+      </c>
+      <c r="M27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1.8</v>
       </c>
@@ -1307,8 +1585,131 @@
       <c r="I28" t="s">
         <v>31</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28">
+        <v>1.6</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>250</v>
+      </c>
+      <c r="M28" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B29">
+        <v>0.3</v>
+      </c>
+      <c r="C29">
+        <v>250</v>
+      </c>
+      <c r="D29">
+        <v>25</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="H29">
+        <v>10</v>
+      </c>
+      <c r="I29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29">
+        <v>1E-3</v>
+      </c>
+      <c r="K29">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="L29">
+        <v>580</v>
+      </c>
+      <c r="M29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B30">
+        <v>0.3</v>
+      </c>
+      <c r="C30">
+        <v>250</v>
+      </c>
+      <c r="D30">
+        <v>25</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <v>10</v>
+      </c>
+      <c r="I30" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30">
+        <v>1E-3</v>
+      </c>
+      <c r="K30">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="L30">
+        <v>580</v>
+      </c>
+      <c r="M30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B31">
+        <v>0.3</v>
+      </c>
+      <c r="C31">
+        <v>250</v>
+      </c>
+      <c r="D31">
+        <v>25</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <v>10</v>
+      </c>
+      <c r="I31" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31">
+        <v>1E-3</v>
+      </c>
+      <c r="K31">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="L31">
+        <v>580</v>
+      </c>
+      <c r="M31" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1318,24 +1719,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[TASK] Improves the topology mutation algorithm
</commit_message>
<xml_diff>
--- a/Experiments/TicTacToe/log.xlsx
+++ b/Experiments/TicTacToe/log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
   <si>
     <t>Mut</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t>nach ca 47 M Comp. Mit minimaler neuron count =&gt; 1.0 rating</t>
+  </si>
+  <si>
+    <t>nach 50 M Comp =&gt; 1.0 rating mit 18-6-4-9 netz</t>
+  </si>
+  <si>
+    <t>nach 46 M Comp =&gt; 1.0 rating mit 18-9-6-9 netz</t>
+  </si>
+  <si>
+    <t>0.07</t>
+  </si>
+  <si>
+    <t>nach 60 M Comp =&gt; 1.0 rating mit 18-9-3-9 netz</t>
   </si>
 </sst>
 </file>
@@ -480,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1710,6 +1722,123 @@
       </c>
       <c r="M31" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B32">
+        <v>0.3</v>
+      </c>
+      <c r="C32">
+        <v>250</v>
+      </c>
+      <c r="D32">
+        <v>25</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>30</v>
+      </c>
+      <c r="J32">
+        <v>1E-3</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>580</v>
+      </c>
+      <c r="M32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B33">
+        <v>0.3</v>
+      </c>
+      <c r="C33">
+        <v>250</v>
+      </c>
+      <c r="D33">
+        <v>25</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>30</v>
+      </c>
+      <c r="J33">
+        <v>1E-3</v>
+      </c>
+      <c r="K33">
+        <v>1E-4</v>
+      </c>
+      <c r="L33">
+        <v>580</v>
+      </c>
+      <c r="M33" t="s">
+        <v>40</v>
+      </c>
+      <c r="N33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B34">
+        <v>0.3</v>
+      </c>
+      <c r="C34">
+        <v>250</v>
+      </c>
+      <c r="D34">
+        <v>25</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>30</v>
+      </c>
+      <c r="J34">
+        <v>1E-3</v>
+      </c>
+      <c r="K34">
+        <v>1E-3</v>
+      </c>
+      <c r="L34">
+        <v>580</v>
+      </c>
+      <c r="M34" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[TASK] The PhasedTopologyMutation does now also add neurons to the mpc calculation
</commit_message>
<xml_diff>
--- a/Experiments/TicTacToe/log.xlsx
+++ b/Experiments/TicTacToe/log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>Mut</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>nach 60 M Comp =&gt; 1.0 rating mit 18-9-3-9 netz</t>
+  </si>
+  <si>
+    <t>nach 58 M Comp =&gt; 1.0 rating mit 18-5-5-9 netz</t>
+  </si>
+  <si>
+    <t>0.05 (phased)</t>
   </si>
 </sst>
 </file>
@@ -492,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1839,6 +1845,47 @@
       </c>
       <c r="M34" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B35">
+        <v>0.3</v>
+      </c>
+      <c r="C35">
+        <v>250</v>
+      </c>
+      <c r="D35">
+        <v>25</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35">
+        <v>1.6</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>580</v>
+      </c>
+      <c r="M35" t="s">
+        <v>43</v>
+      </c>
+      <c r="N35" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>